<commit_message>
Latest code we got in February 2024
</commit_message>
<xml_diff>
--- a/ed-egr-app-develop/src/test-utils/resources/Testfaelle_alte_Routine3.xlsx
+++ b/ed-egr-app-develop/src/test-utils/resources/Testfaelle_alte_Routine3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
   <workbookPr codeName="DieseArbeitsmappe"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\twestphal\project\ed-egr-app\src\test-utils\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C65E4E0D-1286-4582-8294-B68B6CD9FCE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{630B0F9F-C422-4BAB-BC1C-89F59B8EBC6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="940" yWindow="-110" windowWidth="37570" windowHeight="21820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="970" yWindow="-110" windowWidth="18340" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3119" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3120" uniqueCount="153">
   <si>
     <t>Geburtsdatum</t>
   </si>
@@ -492,6 +492,9 @@
   <si>
     <t>Zwischenergebnis aus der alten Java Implementierung</t>
   </si>
+  <si>
+    <t>Angepasst wegen Änderung Steuerberechnung</t>
+  </si>
 </sst>
 </file>
 
@@ -549,7 +552,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -580,6 +583,12 @@
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -642,7 +651,7 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -672,6 +681,8 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="5" applyFill="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="60 % - Akzent5" xfId="5" builtinId="48"/>
@@ -958,12 +969,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Tabelle1"/>
-  <dimension ref="A1:BI156"/>
+  <dimension ref="A1:BI157"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A96" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="A124" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="H1" activePane="topRight" state="frozen"/>
       <selection activeCell="A98" sqref="A98"/>
-      <selection pane="topRight" activeCell="B143" sqref="B143"/>
+      <selection pane="topRight" activeCell="I144" sqref="I144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -23759,11 +23770,11 @@
       <c r="G140">
         <v>855.17</v>
       </c>
-      <c r="H140">
-        <v>1943.09</v>
-      </c>
-      <c r="I140">
-        <v>1264.33</v>
+      <c r="H140" s="17">
+        <v>1937.34</v>
+      </c>
+      <c r="I140" s="17">
+        <v>1256.42</v>
       </c>
       <c r="J140">
         <f>477.51-0.01</f>
@@ -23779,21 +23790,20 @@
         <f>284.7-0.01</f>
         <v>284.69</v>
       </c>
-      <c r="N140">
-        <v>1719.31</v>
-      </c>
-      <c r="O140">
-        <v>1364.26</v>
+      <c r="N140" s="17">
+        <v>1713.15</v>
+      </c>
+      <c r="O140" s="17">
+        <v>1358.68</v>
       </c>
       <c r="P140">
         <v>412.87</v>
       </c>
-      <c r="Q140">
-        <f>1997.16-0.01</f>
-        <v>1997.15</v>
-      </c>
-      <c r="R140">
-        <v>1654.43</v>
+      <c r="Q140" s="17">
+        <v>1990.96</v>
+      </c>
+      <c r="R140" s="17">
+        <v>1648.68</v>
       </c>
       <c r="S140">
         <v>1612.17</v>
@@ -23807,8 +23817,8 @@
       <c r="V140">
         <v>1467.04</v>
       </c>
-      <c r="W140">
-        <v>2213.19</v>
+      <c r="W140" s="17">
+        <v>2207.44</v>
       </c>
       <c r="X140">
         <v>569.6</v>
@@ -23816,14 +23826,14 @@
       <c r="Y140">
         <v>680.51</v>
       </c>
-      <c r="Z140">
-        <v>1555.74</v>
+      <c r="Z140" s="17">
+        <v>1549.99</v>
       </c>
       <c r="AA140">
         <v>1227.8399999999999</v>
       </c>
-      <c r="AB140">
-        <v>2093.37</v>
+      <c r="AB140" s="17">
+        <v>2087.1799999999998</v>
       </c>
       <c r="AC140">
         <v>1886.8</v>
@@ -23834,8 +23844,8 @@
       <c r="AE140" s="16">
         <v>650.80999999999995</v>
       </c>
-      <c r="AF140">
-        <v>1348.42</v>
+      <c r="AF140" s="17">
+        <v>1342.67</v>
       </c>
       <c r="AG140">
         <f>96.12-0.01</f>
@@ -23844,11 +23854,11 @@
       <c r="AH140">
         <v>760.67</v>
       </c>
-      <c r="AI140">
-        <v>1891.17</v>
-      </c>
-      <c r="AJ140">
-        <v>1379.4</v>
+      <c r="AI140" s="17">
+        <v>1885.42</v>
+      </c>
+      <c r="AJ140" s="17">
+        <v>1371.47</v>
       </c>
       <c r="AK140">
         <v>867.67</v>
@@ -23859,8 +23869,8 @@
       <c r="AM140" s="16">
         <v>752.25</v>
       </c>
-      <c r="AN140">
-        <v>1267.0999999999999</v>
+      <c r="AN140" s="17">
+        <v>1261.3499999999999</v>
       </c>
       <c r="AO140" s="16">
         <v>384.17</v>
@@ -23871,8 +23881,8 @@
       <c r="AQ140">
         <v>0</v>
       </c>
-      <c r="AR140">
-        <v>1354.98</v>
+      <c r="AR140" s="17">
+        <v>1347.15</v>
       </c>
       <c r="AS140">
         <v>945.17</v>
@@ -23948,11 +23958,11 @@
       <c r="G141">
         <v>300</v>
       </c>
-      <c r="H141">
-        <v>537.49</v>
-      </c>
-      <c r="I141">
-        <v>978.69</v>
+      <c r="H141" s="17">
+        <v>541.23</v>
+      </c>
+      <c r="I141" s="17">
+        <v>983.83</v>
       </c>
       <c r="J141">
         <v>300</v>
@@ -23966,20 +23976,20 @@
       <c r="M141">
         <v>300</v>
       </c>
-      <c r="N141">
-        <v>448.75</v>
-      </c>
-      <c r="O141">
-        <v>621.20000000000005</v>
+      <c r="N141" s="17">
+        <v>452.76</v>
+      </c>
+      <c r="O141" s="17">
+        <v>624.83000000000004</v>
       </c>
       <c r="P141">
         <v>300</v>
       </c>
-      <c r="Q141">
-        <v>502.35</v>
-      </c>
-      <c r="R141">
-        <v>452.02</v>
+      <c r="Q141" s="17">
+        <v>506.38</v>
+      </c>
+      <c r="R141" s="17">
+        <v>455.76</v>
       </c>
       <c r="S141">
         <v>300</v>
@@ -23993,8 +24003,8 @@
       <c r="V141">
         <v>846.92</v>
       </c>
-      <c r="W141">
-        <v>361.93</v>
+      <c r="W141" s="17">
+        <v>365.66</v>
       </c>
       <c r="X141">
         <v>300</v>
@@ -24002,14 +24012,14 @@
       <c r="Y141">
         <v>595.17999999999995</v>
       </c>
-      <c r="Z141">
-        <v>420.51</v>
+      <c r="Z141" s="17">
+        <v>424.25</v>
       </c>
       <c r="AA141">
         <v>300</v>
       </c>
-      <c r="AB141">
-        <v>439.81</v>
+      <c r="AB141" s="17">
+        <v>443.83</v>
       </c>
       <c r="AC141">
         <v>300</v>
@@ -24020,8 +24030,8 @@
       <c r="AE141" s="16">
         <v>332.13</v>
       </c>
-      <c r="AF141">
-        <v>924.03</v>
+      <c r="AF141" s="17">
+        <v>927.76</v>
       </c>
       <c r="AG141">
         <v>300</v>
@@ -24029,11 +24039,11 @@
       <c r="AH141">
         <v>300</v>
       </c>
-      <c r="AI141">
-        <v>571.24</v>
-      </c>
-      <c r="AJ141">
-        <v>903.89</v>
+      <c r="AI141" s="17">
+        <v>574.98</v>
+      </c>
+      <c r="AJ141" s="17">
+        <v>909.04</v>
       </c>
       <c r="AK141">
         <v>300</v>
@@ -24044,8 +24054,8 @@
       <c r="AM141">
         <v>300</v>
       </c>
-      <c r="AN141">
-        <v>976.89</v>
+      <c r="AN141" s="17">
+        <v>980.62</v>
       </c>
       <c r="AO141" s="16">
         <v>531.95000000000005</v>
@@ -24056,8 +24066,8 @@
       <c r="AQ141">
         <v>0</v>
       </c>
-      <c r="AR141">
-        <v>919.76</v>
+      <c r="AR141" s="17">
+        <v>924.85</v>
       </c>
       <c r="AS141">
         <v>300</v>
@@ -24321,8 +24331,8 @@
       <c r="H143">
         <v>1305.17</v>
       </c>
-      <c r="I143">
-        <v>1189.43</v>
+      <c r="I143" s="17">
+        <v>1181.5999999999999</v>
       </c>
       <c r="J143">
         <v>323.63</v>
@@ -24336,8 +24346,8 @@
       <c r="M143">
         <v>240.6</v>
       </c>
-      <c r="N143">
-        <v>1339.55</v>
+      <c r="N143" s="17">
+        <v>1333.8</v>
       </c>
       <c r="O143">
         <v>1134.8499999999999</v>
@@ -24345,11 +24355,11 @@
       <c r="P143">
         <v>167.22</v>
       </c>
-      <c r="Q143">
-        <v>1622.2</v>
-      </c>
-      <c r="R143">
-        <v>1445.01</v>
+      <c r="Q143" s="17">
+        <v>1616.45</v>
+      </c>
+      <c r="R143" s="17">
+        <v>1439.26</v>
       </c>
       <c r="S143">
         <v>1390.1</v>
@@ -24363,8 +24373,8 @@
       <c r="V143">
         <v>1143.6500000000001</v>
       </c>
-      <c r="W143">
-        <v>1873.04</v>
+      <c r="W143" s="17">
+        <v>1867.29</v>
       </c>
       <c r="X143">
         <v>349.5</v>
@@ -24372,14 +24382,14 @@
       <c r="Y143">
         <v>635.37</v>
       </c>
-      <c r="Z143" s="16">
-        <v>1033.81</v>
+      <c r="Z143" s="18">
+        <v>1029.3900000000001</v>
       </c>
       <c r="AA143">
         <v>1594.67</v>
       </c>
-      <c r="AB143">
-        <v>1682.66</v>
+      <c r="AB143" s="17">
+        <v>1676.91</v>
       </c>
       <c r="AC143">
         <v>1074.49</v>
@@ -24402,8 +24412,8 @@
       <c r="AI143">
         <v>1328.67</v>
       </c>
-      <c r="AJ143">
-        <v>1113.53</v>
+      <c r="AJ143" s="17">
+        <v>1105.7</v>
       </c>
       <c r="AK143">
         <v>557.34</v>
@@ -24414,8 +24424,8 @@
       <c r="AM143" s="16">
         <v>484.64</v>
       </c>
-      <c r="AN143">
-        <v>1293.53</v>
+      <c r="AN143" s="17">
+        <v>1287.78</v>
       </c>
       <c r="AO143">
         <v>547.39</v>
@@ -24426,8 +24436,8 @@
       <c r="AQ143">
         <v>1439.75</v>
       </c>
-      <c r="AR143">
-        <v>990.28</v>
+      <c r="AR143" s="17">
+        <v>986.05</v>
       </c>
       <c r="AS143">
         <v>727.6</v>
@@ -24435,8 +24445,8 @@
       <c r="AT143">
         <v>644.03</v>
       </c>
-      <c r="AU143">
-        <v>1260.71</v>
+      <c r="AU143" s="17">
+        <v>1255.54</v>
       </c>
       <c r="AV143">
         <v>977.25</v>
@@ -24459,17 +24469,17 @@
       <c r="BB143" s="16">
         <v>370.16</v>
       </c>
-      <c r="BC143">
-        <v>1116.32</v>
-      </c>
-      <c r="BD143">
-        <v>1650.92</v>
+      <c r="BC143" s="17">
+        <v>1111.07</v>
+      </c>
+      <c r="BD143" s="17">
+        <v>1645.17</v>
       </c>
       <c r="BE143">
         <v>751.21</v>
       </c>
-      <c r="BF143">
-        <v>1576.65</v>
+      <c r="BF143" s="17">
+        <v>1570.46</v>
       </c>
       <c r="BG143">
         <v>534.22</v>
@@ -24521,8 +24531,8 @@
       <c r="M144">
         <v>196.44</v>
       </c>
-      <c r="N144">
-        <v>695.6</v>
+      <c r="N144" s="17">
+        <v>699.34</v>
       </c>
       <c r="O144">
         <v>753.99</v>
@@ -24530,11 +24540,11 @@
       <c r="P144">
         <v>150</v>
       </c>
-      <c r="Q144">
-        <v>746.07</v>
-      </c>
-      <c r="R144">
-        <v>588.14</v>
+      <c r="Q144" s="17">
+        <v>749.81</v>
+      </c>
+      <c r="R144" s="17">
+        <v>591.88</v>
       </c>
       <c r="S144">
         <v>150</v>
@@ -24548,8 +24558,8 @@
       <c r="V144">
         <v>900</v>
       </c>
-      <c r="W144">
-        <v>583.02</v>
+      <c r="W144" s="17">
+        <v>586.76</v>
       </c>
       <c r="X144">
         <v>298.94</v>
@@ -24563,8 +24573,8 @@
       <c r="AA144">
         <v>150</v>
       </c>
-      <c r="AB144">
-        <v>706.77</v>
+      <c r="AB144" s="17">
+        <v>710.51</v>
       </c>
       <c r="AC144">
         <v>150</v>
@@ -24620,8 +24630,8 @@
       <c r="AT144">
         <v>150</v>
       </c>
-      <c r="AU144">
-        <v>449.97</v>
+      <c r="AU144" s="17">
+        <v>453.33</v>
       </c>
       <c r="AV144">
         <v>150</v>
@@ -24644,17 +24654,17 @@
       <c r="BB144">
         <v>150</v>
       </c>
-      <c r="BC144">
-        <v>297.93</v>
-      </c>
-      <c r="BD144">
-        <v>727.4</v>
+      <c r="BC144" s="17">
+        <v>301.33999999999997</v>
+      </c>
+      <c r="BD144" s="17">
+        <v>731.14</v>
       </c>
       <c r="BE144">
         <v>264.64999999999998</v>
       </c>
-      <c r="BF144">
-        <v>688.35</v>
+      <c r="BF144" s="17">
+        <v>692.37</v>
       </c>
       <c r="BG144">
         <v>150</v>
@@ -25126,11 +25136,11 @@
       </c>
       <c r="H148">
         <f t="shared" si="2"/>
-        <v>84.669999999999845</v>
+        <v>78.919999999999845</v>
       </c>
       <c r="I148">
         <f t="shared" si="2"/>
-        <v>67.959999999999809</v>
+        <v>60.049999999999955</v>
       </c>
       <c r="J148">
         <f t="shared" si="2"/>
@@ -25150,11 +25160,11 @@
       </c>
       <c r="N148">
         <f t="shared" si="2"/>
-        <v>58.259999999999991</v>
+        <v>52.100000000000136</v>
       </c>
       <c r="O148">
         <f t="shared" si="2"/>
-        <v>87.590000000000146</v>
+        <v>82.010000000000218</v>
       </c>
       <c r="P148">
         <f t="shared" si="2"/>
@@ -25162,11 +25172,11 @@
       </c>
       <c r="Q148">
         <f t="shared" si="2"/>
-        <v>85.310000000000173</v>
+        <v>79.120000000000118</v>
       </c>
       <c r="R148">
         <f t="shared" si="1"/>
-        <v>38.840000000000146</v>
+        <v>33.090000000000146</v>
       </c>
       <c r="S148">
         <f t="shared" si="1"/>
@@ -25186,7 +25196,7 @@
       </c>
       <c r="W148">
         <f t="shared" si="1"/>
-        <v>131.76999999999998</v>
+        <v>126.01999999999998</v>
       </c>
       <c r="X148">
         <f t="shared" si="1"/>
@@ -25198,7 +25208,7 @@
       </c>
       <c r="Z148">
         <f t="shared" si="1"/>
-        <v>54.660000000000082</v>
+        <v>48.910000000000082</v>
       </c>
       <c r="AA148">
         <f t="shared" si="1"/>
@@ -25206,7 +25216,7 @@
       </c>
       <c r="AB148">
         <f t="shared" si="1"/>
-        <v>74.909999999999854</v>
+        <v>68.7199999999998</v>
       </c>
       <c r="AC148">
         <f t="shared" si="1"/>
@@ -25222,7 +25232,7 @@
       </c>
       <c r="AF148">
         <f t="shared" si="1"/>
-        <v>52.700000000000045</v>
+        <v>46.950000000000045</v>
       </c>
       <c r="AG148">
         <f t="shared" si="1"/>
@@ -25234,11 +25244,11 @@
       </c>
       <c r="AI148">
         <f t="shared" si="1"/>
-        <v>83.75</v>
+        <v>78</v>
       </c>
       <c r="AJ148">
         <f t="shared" si="1"/>
-        <v>56.310000000000173</v>
+        <v>48.380000000000109</v>
       </c>
       <c r="AK148">
         <f t="shared" si="1"/>
@@ -25254,7 +25264,7 @@
       </c>
       <c r="AN148">
         <f t="shared" si="1"/>
-        <v>47.929999999999836</v>
+        <v>42.179999999999836</v>
       </c>
       <c r="AO148">
         <f t="shared" si="1"/>
@@ -25270,7 +25280,7 @@
       </c>
       <c r="AR148">
         <f t="shared" si="1"/>
-        <v>58.179999999999836</v>
+        <v>50.349999999999909</v>
       </c>
       <c r="AS148">
         <f t="shared" si="1"/>
@@ -25371,11 +25381,11 @@
       </c>
       <c r="H149">
         <f t="shared" si="1"/>
-        <v>-55.039999999999964</v>
+        <v>-51.299999999999955</v>
       </c>
       <c r="I149">
         <f t="shared" si="1"/>
-        <v>-44.169999999999959</v>
+        <v>-39.029999999999973</v>
       </c>
       <c r="J149">
         <f t="shared" si="1"/>
@@ -25395,11 +25405,11 @@
       </c>
       <c r="N149">
         <f t="shared" si="1"/>
-        <v>-37.870000000000005</v>
+        <v>-33.860000000000014</v>
       </c>
       <c r="O149">
         <f t="shared" si="1"/>
-        <v>-56.92999999999995</v>
+        <v>-53.299999999999955</v>
       </c>
       <c r="P149">
         <f t="shared" si="1"/>
@@ -25407,11 +25417,11 @@
       </c>
       <c r="Q149">
         <f t="shared" si="1"/>
-        <v>-55.449999999999932</v>
+        <v>-51.419999999999959</v>
       </c>
       <c r="R149">
         <f t="shared" si="1"/>
-        <v>-25.25</v>
+        <v>-21.509999999999991</v>
       </c>
       <c r="S149">
         <f t="shared" si="1"/>
@@ -25431,7 +25441,7 @@
       </c>
       <c r="W149">
         <f t="shared" si="1"/>
-        <v>-85.649999999999977</v>
+        <v>-81.919999999999959</v>
       </c>
       <c r="X149">
         <f t="shared" si="1"/>
@@ -25443,7 +25453,7 @@
       </c>
       <c r="Z149">
         <f t="shared" si="1"/>
-        <v>-35.53000000000003</v>
+        <v>-31.79000000000002</v>
       </c>
       <c r="AA149">
         <f t="shared" si="1"/>
@@ -25451,7 +25461,7 @@
       </c>
       <c r="AB149">
         <f t="shared" si="1"/>
-        <v>-48.69</v>
+        <v>-44.670000000000016</v>
       </c>
       <c r="AC149">
         <f t="shared" si="1"/>
@@ -25467,7 +25477,7 @@
       </c>
       <c r="AF149">
         <f t="shared" si="1"/>
-        <v>-34.25</v>
+        <v>-30.519999999999982</v>
       </c>
       <c r="AG149">
         <f t="shared" si="1"/>
@@ -25479,11 +25489,11 @@
       </c>
       <c r="AI149">
         <f t="shared" si="1"/>
-        <v>-54.439999999999941</v>
+        <v>-50.699999999999932</v>
       </c>
       <c r="AJ149">
         <f t="shared" si="1"/>
-        <v>-36.600000000000023</v>
+        <v>-31.450000000000045</v>
       </c>
       <c r="AK149">
         <f t="shared" si="1"/>
@@ -25499,7 +25509,7 @@
       </c>
       <c r="AN149">
         <f t="shared" si="1"/>
-        <v>-31.149999999999977</v>
+        <v>-27.419999999999959</v>
       </c>
       <c r="AO149">
         <f t="shared" si="1"/>
@@ -25515,7 +25525,7 @@
       </c>
       <c r="AR149">
         <f t="shared" si="1"/>
-        <v>-37.82000000000005</v>
+        <v>-32.730000000000018</v>
       </c>
       <c r="AS149">
         <f t="shared" si="1"/>
@@ -25865,7 +25875,7 @@
       </c>
       <c r="I151">
         <f t="shared" si="1"/>
-        <v>68.490000000000009</v>
+        <v>60.659999999999854</v>
       </c>
       <c r="J151">
         <f t="shared" si="1"/>
@@ -25885,7 +25895,7 @@
       </c>
       <c r="N151">
         <f t="shared" si="1"/>
-        <v>45.249999999999773</v>
+        <v>39.499999999999773</v>
       </c>
       <c r="O151">
         <f t="shared" si="1"/>
@@ -25897,11 +25907,11 @@
       </c>
       <c r="Q151">
         <f t="shared" si="1"/>
-        <v>58.269999999999982</v>
+        <v>52.519999999999982</v>
       </c>
       <c r="R151">
         <f t="shared" si="1"/>
-        <v>37.25</v>
+        <v>31.5</v>
       </c>
       <c r="S151">
         <f t="shared" si="1"/>
@@ -25921,7 +25931,7 @@
       </c>
       <c r="W151">
         <f t="shared" si="1"/>
-        <v>107.82999999999993</v>
+        <v>102.07999999999993</v>
       </c>
       <c r="X151">
         <f t="shared" si="1"/>
@@ -25933,7 +25943,7 @@
       </c>
       <c r="Z151">
         <f t="shared" si="1"/>
-        <v>32.719999999999914</v>
+        <v>28.300000000000068</v>
       </c>
       <c r="AA151">
         <f t="shared" si="1"/>
@@ -25941,7 +25951,7 @@
       </c>
       <c r="AB151">
         <f t="shared" si="1"/>
-        <v>52.689999999999827</v>
+        <v>46.939999999999827</v>
       </c>
       <c r="AC151">
         <f t="shared" si="1"/>
@@ -25973,7 +25983,7 @@
       </c>
       <c r="AJ151">
         <f t="shared" si="1"/>
-        <v>65.379999999999882</v>
+        <v>57.549999999999955</v>
       </c>
       <c r="AK151">
         <f t="shared" ref="C151:BI153" si="3">AK143-AK106</f>
@@ -25989,7 +25999,7 @@
       </c>
       <c r="AN151">
         <f t="shared" si="3"/>
-        <v>48.509999999999991</v>
+        <v>42.759999999999991</v>
       </c>
       <c r="AO151">
         <f t="shared" si="3"/>
@@ -26005,7 +26015,7 @@
       </c>
       <c r="AR151">
         <f t="shared" si="3"/>
-        <v>57.209999999999923</v>
+        <v>52.979999999999905</v>
       </c>
       <c r="AS151">
         <f t="shared" si="3"/>
@@ -26017,7 +26027,7 @@
       </c>
       <c r="AU151">
         <f t="shared" si="3"/>
-        <v>36.090000000000146</v>
+        <v>30.920000000000073</v>
       </c>
       <c r="AV151">
         <f t="shared" si="3"/>
@@ -26049,11 +26059,11 @@
       </c>
       <c r="BC151">
         <f t="shared" si="3"/>
-        <v>37.329999999999927</v>
+        <v>32.079999999999927</v>
       </c>
       <c r="BD151">
         <f t="shared" si="3"/>
-        <v>98.75</v>
+        <v>93</v>
       </c>
       <c r="BE151">
         <f t="shared" si="3"/>
@@ -26061,7 +26071,7 @@
       </c>
       <c r="BF151">
         <f t="shared" si="3"/>
-        <v>65.190000000000055</v>
+        <v>59</v>
       </c>
       <c r="BG151">
         <f t="shared" si="3"/>
@@ -26130,7 +26140,7 @@
       </c>
       <c r="N152">
         <f t="shared" si="3"/>
-        <v>-29.409999999999968</v>
+        <v>-25.669999999999959</v>
       </c>
       <c r="O152">
         <f t="shared" si="3"/>
@@ -26142,11 +26152,11 @@
       </c>
       <c r="Q152">
         <f t="shared" si="3"/>
-        <v>-37.879999999999995</v>
+        <v>-34.1400000000001</v>
       </c>
       <c r="R152">
         <f t="shared" si="3"/>
-        <v>-24.220000000000027</v>
+        <v>-20.480000000000018</v>
       </c>
       <c r="S152">
         <f t="shared" si="3"/>
@@ -26166,7 +26176,7 @@
       </c>
       <c r="W152">
         <f t="shared" si="3"/>
-        <v>-70.090000000000032</v>
+        <v>-66.350000000000023</v>
       </c>
       <c r="X152">
         <f t="shared" si="3"/>
@@ -26186,7 +26196,7 @@
       </c>
       <c r="AB152">
         <f t="shared" si="3"/>
-        <v>-34.25</v>
+        <v>-30.509999999999991</v>
       </c>
       <c r="AC152">
         <f t="shared" si="3"/>
@@ -26262,7 +26272,7 @@
       </c>
       <c r="AU152">
         <f t="shared" si="3"/>
-        <v>-23.45999999999998</v>
+        <v>-20.100000000000023</v>
       </c>
       <c r="AV152">
         <f t="shared" si="3"/>
@@ -26294,11 +26304,11 @@
       </c>
       <c r="BC152">
         <f t="shared" si="3"/>
-        <v>-24.269999999999982</v>
+        <v>-20.860000000000014</v>
       </c>
       <c r="BD152">
         <f t="shared" si="3"/>
-        <v>-64.190000000000055</v>
+        <v>-60.450000000000045</v>
       </c>
       <c r="BE152">
         <f t="shared" si="3"/>
@@ -26306,7 +26316,7 @@
       </c>
       <c r="BF152">
         <f t="shared" si="3"/>
-        <v>-42.370000000000005</v>
+        <v>-38.350000000000023</v>
       </c>
       <c r="BG152">
         <f t="shared" si="3"/>
@@ -26569,6 +26579,11 @@
     <row r="156" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A156" s="16" t="s">
         <v>149</v>
+      </c>
+    </row>
+    <row r="157" spans="1:61" x14ac:dyDescent="0.35">
+      <c r="A157" s="17" t="s">
+        <v>152</v>
       </c>
     </row>
   </sheetData>

</xml_diff>